<commit_message>
added row add, clear workspace; needs the ability to be reactive and update the overlay on the click of the overlay... needs a publish button
</commit_message>
<xml_diff>
--- a/frontend/my-react-app/public/DefaultSchemaSheet.xlsx
+++ b/frontend/my-react-app/public/DefaultSchemaSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>Code</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>TaxonomyDescription</t>
-  </si>
-  <si>
-    <t>dropdown(with types)</t>
   </si>
   <si>
     <t>Prefix</t>
@@ -227,16 +224,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,24 +534,12 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -1590,58 +1572,44 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -2673,64 +2641,48 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -3757,37 +3709,27 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -4818,55 +4760,39 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -5893,31 +5819,23 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -6944,31 +6862,22 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -7998,49 +7907,35 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -9067,31 +8962,23 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -10123,61 +10010,43 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -11203,25 +11072,19 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -12252,55 +12115,39 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -13329,49 +13176,35 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -14401,49 +14234,35 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -15473,55 +15292,39 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>

</xml_diff>